<commit_message>
Improve clarity of correction report
- Each question can have an intelligible title, so students don't have
  to remember what Q2c was about if they don't have the questionaire
  with them

- The table of lost points shows how many points were lost per error AND
  how often each error occured

- Adapted template

 On branch main
 Changes to be committed:
	modified:   template/template_correction_examen.xlsx
	modified:   transparent_correction.py
</commit_message>
<xml_diff>
--- a/template/template_correction_examen.xlsx
+++ b/template/template_correction_examen.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="81">
   <si>
     <t xml:space="preserve">Documentation</t>
   </si>
@@ -161,7 +161,13 @@
     <t xml:space="preserve">questions</t>
   </si>
   <si>
+    <t xml:space="preserve">titre</t>
+  </si>
+  <si>
     <t xml:space="preserve">&lt;+points totaux si tout bon +&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;+ “Nom” de la question / sujet principal +&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;+points avant correction +&gt;</t>
@@ -432,81 +438,65 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
 </styleSheet>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -516,12 +506,12 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14.44"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="16.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="53.72"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="1" width="11.52"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -586,7 +576,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -595,11 +585,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -607,130 +597,130 @@
       <selection pane="bottomLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="54.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.92"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="54.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="18.92"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="5" style="3" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="S1" s="3"/>
-      <c r="T1" s="3"/>
-      <c r="U1" s="3"/>
-      <c r="V1" s="3"/>
-      <c r="W1" s="3"/>
-      <c r="X1" s="3"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4"/>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="4"/>
+      <c r="V1" s="4"/>
+      <c r="W1" s="4"/>
+      <c r="X1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="4" t="n">
+      <c r="D2" s="5" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="4" t="n">
+      <c r="C3" s="5" t="n">
         <v>0.2</v>
       </c>
-      <c r="D3" s="4" t="n">
+      <c r="D3" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="4" t="n">
+      <c r="C4" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C5" s="4" t="n">
+      <c r="C5" s="5" t="n">
         <v>0.1</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="C6" s="4" t="n">
+      <c r="C6" s="5" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C7" s="4" t="n">
+      <c r="C7" s="5" t="n">
         <f aca="false">1/5</f>
         <v>0.2</v>
       </c>
-      <c r="D7" s="4" t="n">
+      <c r="D7" s="5" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="D8" s="4" t="n">
+      <c r="D8" s="5" t="n">
         <v>0.25</v>
       </c>
     </row>
@@ -1728,8 +1718,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -1738,11 +1728,11 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D75"/>
+  <dimension ref="A1:D998"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -1750,70 +1740,70 @@
       <selection pane="bottomLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="21.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="125.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="5" width="19.35"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="11.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="21.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="125.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="19.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="54.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="3" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="7" style="3" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6"/>
-      <c r="B1" s="3" t="s">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9"/>
-      <c r="B3" s="8" t="s">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="5" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="D4" s="10"/>
+      <c r="A4" s="5"/>
+      <c r="D4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2812,8 +2802,8 @@
     <row r="998" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -2822,11 +2812,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G992"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
@@ -2836,66 +2826,66 @@
       <selection pane="bottomRight" activeCell="E1" activeCellId="0" sqref="E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="14.9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="33.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="14.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="21.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="18.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="19.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="13.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="22.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="36.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="18" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.58"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="14.9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="23.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="3" width="33.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="5" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="3" width="15.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="3" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="3" width="21.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="3" width="18.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="3" width="20.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="3" width="19.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="3" width="13.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="3" width="22.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="3" width="36.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="18" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="3" width="17.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="3" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B1" s="11" t="s">
+    <row r="1" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B1" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="C1" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="11" t="s">
+      <c r="D1" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="E1" s="11" t="s">
+      <c r="E1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G1" s="11" t="s">
+      <c r="G1" s="7" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="13" t="s">
+      <c r="B2" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="8"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -3889,8 +3879,8 @@
     <row r="992" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -3899,55 +3889,67 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="27.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="3" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>44</v>
+      <c r="B2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>44</v>
+      <c r="B3" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>44</v>
+      <c r="B4" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -4948,8 +4950,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -4958,11 +4960,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -4970,43 +4972,43 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="5" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="34.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="34.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="3" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
+    <row r="1" s="7" customFormat="true" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>45</v>
+      <c r="B2" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>45</v>
+      <c r="B3" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>45</v>
+      <c r="B4" s="5" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -6007,8 +6009,8 @@
     <row r="1000" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6017,11 +6019,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -6029,56 +6031,56 @@
       <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="46.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="58.2"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="3" width="20.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="46.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="3" width="58.2"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="4" style="3" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="7" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>47</v>
+      <c r="B1" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>49</v>
+      <c r="B2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B3" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>51</v>
+      <c r="B3" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B4" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>53</v>
+      <c r="B4" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6103,8 +6105,8 @@
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>
@@ -6113,7 +6115,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
@@ -6123,130 +6125,130 @@
       <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="11" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="126.74"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="7" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="3" width="126.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="3" width="11.52"/>
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>54</v>
+      <c r="A2" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>56</v>
+      <c r="A5" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="s">
-        <v>57</v>
+      <c r="B6" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="B8" s="0" t="s">
-        <v>59</v>
+      <c r="A8" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11" t="s">
-        <v>60</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>61</v>
+      <c r="A10" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="0" t="s">
-        <v>62</v>
+      <c r="B11" s="3" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>64</v>
+      <c r="A13" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="B15" s="0" t="s">
-        <v>66</v>
+      <c r="A15" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="0" t="s">
-        <v>67</v>
+      <c r="B16" s="3" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="11" t="s">
-        <v>68</v>
+      <c r="A18" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="0" t="s">
-        <v>69</v>
+      <c r="B19" s="3" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="0" t="s">
-        <v>70</v>
+      <c r="B20" s="3" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="B23" s="0" t="s">
-        <v>72</v>
+      <c r="A23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="14" t="s">
-        <v>73</v>
+      <c r="B25" s="10" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="14" t="s">
-        <v>74</v>
+      <c r="B26" s="10" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="14" t="s">
-        <v>75</v>
+      <c r="B27" s="10" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="14" t="s">
-        <v>76</v>
+      <c r="B28" s="10" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="14" t="s">
-        <v>77</v>
+      <c r="B29" s="10" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="83.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="14" t="s">
-        <v>78</v>
+      <c r="B30" s="10" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>